<commit_message>
draft creation of DFBA exchange reactions; test DFBA submodels; remove a list.index() op from sort of simulation events by event priority
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/submodels/fixtures/test_submodel_no_shared_species.xlsx
+++ b/tests/multialgorithm/submodels/fixtures/test_submodel_no_shared_species.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="460" windowWidth="25840" windowHeight="11640" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="-30960" yWindow="1820" windowWidth="28940" windowHeight="13300" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t>Max flux</t>
+  </si>
+  <si>
+    <t>Objective proportion</t>
   </si>
 </sst>
 </file>
@@ -1633,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1648,7 +1651,7 @@
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -1670,8 +1673,11 @@
       <c r="G1" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -1684,13 +1690,16 @@
       <c r="D2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1703,13 +1712,16 @@
       <c r="D3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1722,13 +1734,16 @@
       <c r="D4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1741,13 +1756,16 @@
       <c r="D5" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
@@ -1760,8 +1778,11 @@
       <c r="D6" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="7" t="b">
         <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1779,7 +1800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+    <sheetView zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
give DynamicSubmodels multiple DynamicCompartment add initialization: 	MultialgorithmSimulation.create_dynamic_compartments_for_submodel() Fix DynamicSubmodel methods get_specie_concentrations() & calc_reaction_rates() Fix bug in LocalSpeciesPopulation.__init__() continue renaming sim Submodel to DynamicSubmodel
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/submodels/fixtures/test_submodel_no_shared_species.xlsx
+++ b/tests/multialgorithm/submodels/fixtures/test_submodel_no_shared_species.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="460" yWindow="460" windowWidth="33580" windowHeight="17540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28100" windowHeight="17540" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="126">
   <si>
     <t>ID</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>Objective function</t>
+  </si>
+  <si>
+    <t>max( specie_4[c], 2)</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1730,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="197" zoomScaleNormal="197" zoomScalePageLayoutView="197" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1819,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView zoomScale="148" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1969,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2069,7 +2072,7 @@
         <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="D6" s="6">
         <v>2.9999999999999997E-4</v>

</xml_diff>